<commit_message>
update 2 - added scatter plot
html, excel file and script js all updated
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donald/Downloads/CIS321/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donald/Documents/GitHub/financial-analysis-webapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A3A4D4-DBDC-744D-A911-084AB1B28CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108CBB81-9878-8B46-8E20-D884456967B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{FC06E1C2-8ED8-7744-B4BD-18B0E3A25E62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>sales</t>
   </si>
@@ -47,25 +47,43 @@
     <t>expenses</t>
   </si>
   <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Feb</t>
-  </si>
-  <si>
-    <t>Mar</t>
-  </si>
-  <si>
-    <t>Apr</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>Jun</t>
-  </si>
-  <si>
     <t>month</t>
+  </si>
+  <si>
+    <t>Jan-2023</t>
+  </si>
+  <si>
+    <t>Feb-2023</t>
+  </si>
+  <si>
+    <t>Mar-2023</t>
+  </si>
+  <si>
+    <t>Apr-2023</t>
+  </si>
+  <si>
+    <t>May-2023</t>
+  </si>
+  <si>
+    <t>June-2023</t>
+  </si>
+  <si>
+    <t>July-2023</t>
+  </si>
+  <si>
+    <t>Aug-2023</t>
+  </si>
+  <si>
+    <t>Sep-2023</t>
+  </si>
+  <si>
+    <t>Oct-2023</t>
+  </si>
+  <si>
+    <t>Nov-2023</t>
+  </si>
+  <si>
+    <t>Dec-2023</t>
   </si>
 </sst>
 </file>
@@ -107,8 +125,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,15 +442,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405BE615-7EAD-2D4F-A584-0847F2028F6B}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>9</v>
+      <c r="A1" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -444,78 +468,83 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <f>B2-C2</f>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
+      <c r="A3" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C3">
         <v>18</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <f t="shared" ref="D3:D13" si="0">B3-C3</f>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
+      <c r="A4" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>27</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
+      <c r="A5" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B5">
         <v>40</v>
       </c>
       <c r="C5">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
+      <c r="A6" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="C6">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
+      <c r="A7" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B7">
         <v>60</v>
@@ -524,7 +553,98 @@
         <v>54</v>
       </c>
       <c r="D7">
+        <f t="shared" si="0"/>
         <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>90</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>37</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>36</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>60</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>